<commit_message>
Add clirfication of libraries needed
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gotling/Dev/Sobhana/sensor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E14FCDC-2448-FC48-8C6E-95D7567AF081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC05821-60C3-874B-931E-9CC9ACAE0EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="860" windowWidth="17180" windowHeight="17040" xr2:uid="{59CF69ED-35A2-E747-A272-8368A610B0D4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>D15</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Close Out</t>
   </si>
   <si>
-    <t>OU</t>
-  </si>
-  <si>
     <t>BD</t>
   </si>
   <si>
@@ -205,18 +202,6 @@
   </si>
   <si>
     <t>RX0</t>
-  </si>
-  <si>
-    <t>RPT</t>
-  </si>
-  <si>
-    <t>RPR</t>
-  </si>
-  <si>
-    <t>Raspberry Pi Transmit</t>
-  </si>
-  <si>
-    <t>Raspberry Pi Receive</t>
   </si>
 </sst>
 </file>
@@ -338,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -351,6 +336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF635C60-2181-1942-9BDD-5CAD75B5BA82}">
-  <dimension ref="A3:O21"/>
+  <dimension ref="A3:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:I7"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -702,16 +688,16 @@
       <c r="G3" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="I3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="11" t="s">
         <v>42</v>
       </c>
     </row>
@@ -814,7 +800,7 @@
         <v>24</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>25</v>
@@ -830,36 +816,32 @@
       <c r="A7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="I7" t="s">
-        <v>50</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>58</v>
-      </c>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
@@ -900,42 +882,26 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update pinout for 2 halls
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gotling/Dev/Sobhana/sensor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gotling/Dev/Gotling/window-control/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC05821-60C3-874B-931E-9CC9ACAE0EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C205970D-CAA1-1944-9344-18EC267783A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="860" windowWidth="17180" windowHeight="17040" xr2:uid="{59CF69ED-35A2-E747-A272-8368A610B0D4}"/>
+    <workbookView xWindow="9760" yWindow="2000" windowWidth="20480" windowHeight="17040" xr2:uid="{59CF69ED-35A2-E747-A272-8368A610B0D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>D15</t>
   </si>
@@ -159,30 +159,6 @@
     <t>P3</t>
   </si>
   <si>
-    <t>OI</t>
-  </si>
-  <si>
-    <t>CI</t>
-  </si>
-  <si>
-    <t>Open In</t>
-  </si>
-  <si>
-    <t>Close In</t>
-  </si>
-  <si>
-    <t>OO</t>
-  </si>
-  <si>
-    <t>Open Out</t>
-  </si>
-  <si>
-    <t>CO</t>
-  </si>
-  <si>
-    <t>Close Out</t>
-  </si>
-  <si>
     <t>BD</t>
   </si>
   <si>
@@ -202,6 +178,60 @@
   </si>
   <si>
     <t>RX0</t>
+  </si>
+  <si>
+    <t>O1</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C1O</t>
+  </si>
+  <si>
+    <t>C2O</t>
+  </si>
+  <si>
+    <t>CO1</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>CI1</t>
+  </si>
+  <si>
+    <t>CI2</t>
+  </si>
+  <si>
+    <t>Close In Second hall</t>
+  </si>
+  <si>
+    <t>Close In First hall</t>
+  </si>
+  <si>
+    <t>Close Out First hall</t>
+  </si>
+  <si>
+    <t>Close Out Second hall</t>
+  </si>
+  <si>
+    <t>OI1</t>
+  </si>
+  <si>
+    <t>OI2</t>
+  </si>
+  <si>
+    <t>Open in First Hall</t>
+  </si>
+  <si>
+    <t>Open in Second hall</t>
   </si>
 </sst>
 </file>
@@ -355,7 +385,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -651,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF635C60-2181-1942-9BDD-5CAD75B5BA82}">
-  <dimension ref="A3:O18"/>
+  <dimension ref="A3:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="I2" sqref="I2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,16 +719,16 @@
         <v>34</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -800,7 +830,7 @@
         <v>24</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>25</v>
@@ -832,16 +862,22 @@
         <v>30</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
+      <c r="N7" t="s">
+        <v>53</v>
+      </c>
+      <c r="O7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
@@ -850,58 +886,74 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" t="s">
-        <v>54</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>